<commit_message>
add credential to function argument
</commit_message>
<xml_diff>
--- a/scripts.xlsx
+++ b/scripts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365cmu-my.sharepoint.com/personal/supawat_s_cmu_ac_th/Documents/MyProjects/ppt-auto-voice-embeded-python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365cmu-my.sharepoint.com/personal/supawat_s_cmu_ac_th/Documents/MyProjects/pptx-auto-voice-embeded-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_973893BB67E831A46AC68134DD3698A768728961" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DB08A84-0136-46EB-9FFD-05D863BAEAC4}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_973893BB67E831A46AC68134DD3698A768728961" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6CD81F9-EE9F-4FBC-B6E0-CC1B5A98EC02}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1665" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5565" yWindow="1530" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -315,12 +315,12 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>